<commit_message>
Update: Python scripts and Sample file
</commit_message>
<xml_diff>
--- a/Sample file.xlsx
+++ b/Sample file.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\AG_Abken\Tina\02) ELISA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\Curve-Fitting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,106 +14,49 @@
   <sheets>
     <sheet name="Result sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
-  <si>
-    <t>Method name: Astrid`s ELISA</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Application: SparkControl</t>
-  </si>
-  <si>
-    <t>V2.3</t>
-  </si>
-  <si>
-    <t>Device: Spark 10M</t>
-  </si>
-  <si>
-    <t>Serial number: 1511009826</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t>Firmware:</t>
   </si>
   <si>
-    <t>LUM:V5.2.3|ABS:V4.3.2|ABS_MEX:V5.0.7|MTP:V12.4.0|FLUOR:V5.1.3|FLUOR_MEM:V5.0.7|FLUOR_MEX:V5.0.7</t>
-  </si>
-  <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-11</t>
-  </si>
-  <si>
     <t>Time:</t>
   </si>
   <si>
-    <t>2:09 PM</t>
-  </si>
-  <si>
     <t>System</t>
   </si>
   <si>
-    <t>PC80015</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
-    <t>PC80015\INSTR-USER</t>
-  </si>
-  <si>
     <t>Plate</t>
   </si>
   <si>
-    <t>[NUN96ft] - Thermo Fisher Scientific-Nunclon 96 Flat Transparent Catalog No.: 269620/269787/439454/442404/475094</t>
-  </si>
-  <si>
     <t>Lid lifter</t>
   </si>
   <si>
-    <t>No lid</t>
-  </si>
-  <si>
     <t>Humidity Cassette</t>
   </si>
   <si>
-    <t>No humidity cassette</t>
-  </si>
-  <si>
     <t>Smooth mode</t>
   </si>
   <si>
-    <t>Selected</t>
-  </si>
-  <si>
     <t>List of actions in this measurement script:</t>
   </si>
   <si>
-    <t>Shaking</t>
-  </si>
-  <si>
     <t>Absorbance</t>
   </si>
   <si>
-    <t>ABTS</t>
-  </si>
-  <si>
-    <t>Move plate</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>NUN96ft</t>
-  </si>
-  <si>
     <t>Plate layout</t>
   </si>
   <si>
@@ -126,39 +69,21 @@
     <t>Start Time</t>
   </si>
   <si>
-    <t>2023-05-11 14:08:36</t>
-  </si>
-  <si>
     <t>Shaking (Linear) Duration</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Shaking (Linear) Position</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
     <t>Shaking (Linear) Amplitude</t>
   </si>
   <si>
-    <t>mm</t>
-  </si>
-  <si>
     <t>Shaking (Linear) Frequency</t>
   </si>
   <si>
-    <t>rpm</t>
-  </si>
-  <si>
     <t>End Time</t>
   </si>
   <si>
-    <t>2023-05-11 14:08:41</t>
-  </si>
-  <si>
     <t>Mode</t>
   </si>
   <si>
@@ -183,9 +108,6 @@
     <t>Part of Plate</t>
   </si>
   <si>
-    <t>2023-05-11 14:08:44</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
@@ -261,16 +183,22 @@
     <t>Difference</t>
   </si>
   <si>
-    <t>2023-05-11 14:09:47</t>
-  </si>
-  <si>
     <t>Movement</t>
   </si>
   <si>
-    <t>Out</t>
-  </si>
-  <si>
-    <t>2023-05-11 14:09:59</t>
+    <t>Method name: Lorem ipsum</t>
+  </si>
+  <si>
+    <t>Application: Lorem ipsum</t>
+  </si>
+  <si>
+    <t>Device: Lorem ipsum</t>
+  </si>
+  <si>
+    <t>Serial number: Lorem ipsum</t>
+  </si>
+  <si>
+    <t>Lorem ipsum</t>
   </si>
 </sst>
 </file>
@@ -326,10 +254,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -636,22 +564,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:M76"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -661,14 +587,12 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -678,13 +602,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -695,13 +619,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -711,15 +635,11 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -729,13 +649,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -746,13 +666,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -763,13 +683,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -780,13 +700,13 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -797,13 +717,13 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -814,13 +734,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -831,13 +751,13 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -848,13 +768,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -878,7 +798,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -893,7 +813,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -909,7 +829,7 @@
     <row r="17" spans="1:11">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -924,15 +844,13 @@
     <row r="18" spans="1:11">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -941,7 +859,7 @@
     <row r="19" spans="1:11">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -968,13 +886,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -985,7 +903,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1000,13 +918,13 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1030,13 +948,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1047,17 +965,15 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="E26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1066,13 +982,13 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1083,17 +999,15 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="E28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1102,17 +1016,15 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1">
-        <v>1440</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="E29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1121,13 +1033,13 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1151,10 +1063,10 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1168,10 +1080,10 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1185,16 +1097,16 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1">
-        <v>405</v>
+      <c r="E34" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1204,16 +1116,16 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1">
-        <v>490</v>
+      <c r="E35" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -1223,13 +1135,13 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1">
-        <v>10</v>
+      <c r="E36" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1240,16 +1152,16 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="1">
-        <v>50</v>
+      <c r="E37" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -1259,13 +1171,13 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1289,13 +1201,13 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1306,16 +1218,16 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1">
-        <v>23.2</v>
+      <c r="E41" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -1338,7 +1250,7 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1353,48 +1265,48 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="3" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1">
         <v>0.64159999999999995</v>
@@ -1435,7 +1347,7 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>0.51970000000000005</v>
@@ -1476,7 +1388,7 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="3" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>0.65300000000000002</v>
@@ -1517,7 +1429,7 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="3" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>0.18379999999999999</v>
@@ -1558,7 +1470,7 @@
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="3" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>0.68600000000000005</v>
@@ -1599,7 +1511,7 @@
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="3" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>0.26860000000000001</v>
@@ -1640,7 +1552,7 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1">
         <v>0.70730000000000004</v>
@@ -1681,7 +1593,7 @@
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="3" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1">
         <v>0.73850000000000005</v>
@@ -1748,7 +1660,7 @@
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1763,48 +1675,48 @@
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="3" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B57" s="1">
         <v>0.10290000000000001</v>
@@ -1845,7 +1757,7 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="B58" s="1">
         <v>9.2700000000000005E-2</v>
@@ -1886,7 +1798,7 @@
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="3" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="B59" s="1">
         <v>0.10349999999999999</v>
@@ -1927,7 +1839,7 @@
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="3" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B60" s="1">
         <v>5.5899999999999998E-2</v>
@@ -1968,7 +1880,7 @@
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="3" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B61" s="1">
         <v>0.1032</v>
@@ -2009,7 +1921,7 @@
     </row>
     <row r="62" spans="1:13">
       <c r="A62" s="3" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B62" s="1">
         <v>6.3500000000000001E-2</v>
@@ -2050,7 +1962,7 @@
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="B63" s="1">
         <v>0.10349999999999999</v>
@@ -2091,7 +2003,7 @@
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="3" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B64" s="1">
         <v>0.1095</v>
@@ -2158,7 +2070,7 @@
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="1" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2173,48 +2085,48 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="3" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B69" s="1">
         <v>0.53869999999999996</v>
@@ -2255,7 +2167,7 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="B70" s="1">
         <v>0.42699999999999999</v>
@@ -2296,7 +2208,7 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="3" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="B71" s="1">
         <v>0.54949999999999999</v>
@@ -2337,7 +2249,7 @@
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="3" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B72" s="1">
         <v>0.12790000000000001</v>
@@ -2378,7 +2290,7 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="3" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B73" s="1">
         <v>0.58279999999999998</v>
@@ -2419,7 +2331,7 @@
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="3" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B74" s="1">
         <v>0.2051</v>
@@ -2460,7 +2372,7 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="B75" s="1">
         <v>0.6038</v>
@@ -2501,7 +2413,7 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="3" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B76" s="1">
         <v>0.629</v>
@@ -2568,13 +2480,13 @@
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -2598,13 +2510,13 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -2615,13 +2527,13 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>

</xml_diff>